<commit_message>
removed bunny font link
</commit_message>
<xml_diff>
--- a/storage/app/public/books.xlsx
+++ b/storage/app/public/books.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="142">
   <si>
     <t xml:space="preserve">Title</t>
   </si>
@@ -55,9 +55,6 @@
     <t xml:space="preserve">Nathan W. Shaw</t>
   </si>
   <si>
-    <t xml:space="preserve">https://plus.unsplash.com/premium_photo-1674068280903-0573fc9358ab?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwxfHx8ZW58MHx8fHx8</t>
-  </si>
-  <si>
     <t xml:space="preserve">Flowers</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
     <t xml:space="preserve">John A. Harper</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1739481913094-b85f7bdabf77?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwyfHx8ZW58MHx8fHx8</t>
-  </si>
-  <si>
     <t xml:space="preserve">Boom the Board</t>
   </si>
   <si>
@@ -91,9 +85,6 @@
     <t xml:space="preserve">Michael T. Fisher</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1739477021967-e14dc3938e56?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwzfHx8ZW58MHx8fHx8</t>
-  </si>
-  <si>
     <t xml:space="preserve">A tiger beside the river</t>
   </si>
   <si>
@@ -109,9 +100,6 @@
     <t xml:space="preserve">Emily R. Dawson</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1736604860264-e2f21df57a89?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHw2fHx8ZW58MHx8fHx8</t>
-  </si>
-  <si>
     <t xml:space="preserve">The driver and the passanger</t>
   </si>
   <si>
@@ -124,9 +112,6 @@
     <t xml:space="preserve">1816659225151</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1739455146717-4f05b6f2d2ec?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHw0fHx8ZW58MHx8fHx8</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gold rod</t>
   </si>
   <si>
@@ -142,9 +127,6 @@
     <t xml:space="preserve">Sophia K. Ellis</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1737304697097-62a820f71964?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHw3fHx8ZW58MHx8fHx8</t>
-  </si>
-  <si>
     <t xml:space="preserve">The red girl</t>
   </si>
   <si>
@@ -157,9 +139,6 @@
     <t xml:space="preserve">4922725558767</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1738071545459-e19435ae37e0?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwxMHx8fGVufDB8fHx8fA%3D%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">Very forgotten</t>
   </si>
   <si>
@@ -169,9 +148,6 @@
     <t xml:space="preserve">5798277762912</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1738168279272-c08d6dd22002?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwxMXx8fGVufDB8fHx8fA%3D%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">The Lost Horizon</t>
   </si>
   <si>
@@ -184,9 +160,6 @@
     <t xml:space="preserve">9599936269273</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1738682081595-7bac257f60cd?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwxNXx8fGVufDB8fHx8fA%3D%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">The Enchanted Voyage</t>
   </si>
   <si>
@@ -199,9 +172,6 @@
     <t xml:space="preserve">Isabella M. Carter</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1739486549895-c1e03729a253?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwyNnx8fGVufDB8fHx8fA%3D%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">Legends of the Forgotten</t>
   </si>
   <si>
@@ -214,9 +184,6 @@
     <t xml:space="preserve">Laura P. Bennett</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1739467444239-840b9b3c2480?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwyOHx8fGVufDB8fHx8fA%3D%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">Beyond the Stars</t>
   </si>
   <si>
@@ -229,9 +196,6 @@
     <t xml:space="preserve">Robert J. Sinclair</t>
   </si>
   <si>
-    <t xml:space="preserve">https://plus.unsplash.com/premium_photo-1739037172419-98ead2ee574f?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwzM3x8fGVufDB8fHx8fA%3D%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">Whispers in the Wind</t>
   </si>
   <si>
@@ -241,9 +205,6 @@
     <t xml:space="preserve">2848286684408</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1739208682228-0a3f71db04de?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHw1OHx8fGVufDB8fHx8fA%3D%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mysteries Unraveled</t>
   </si>
   <si>
@@ -253,24 +214,15 @@
     <t xml:space="preserve">Olivia G. Clarke</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1739388845093-e1d4069cb6b8?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHw1OXx8fGVufDB8fHx8fA%3D%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">8602049495893</t>
   </si>
   <si>
-    <t xml:space="preserve">https://plus.unsplash.com/premium_photo-1739091068170-5486fbb36cff?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHw2NXx8fGVufDB8fHx8fA%3D%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">245</t>
   </si>
   <si>
     <t xml:space="preserve">3320207556626</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1738969773091-abcf274f7e0a?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwyMDN8fHxlbnwwfHx8fHw%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">A Tale of Two Realms</t>
   </si>
   <si>
@@ -280,9 +232,6 @@
     <t xml:space="preserve">1758097791616</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1738760479351-b25b4e35106a?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwyMDl8fHxlbnwwfHx8fHw%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">Boring the job</t>
   </si>
   <si>
@@ -292,9 +241,6 @@
     <t xml:space="preserve">1184614337908</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1738676524296-364cf18900a8?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwyMjB8fHxlbnwwfHx8fHw%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">Echoes of the Past</t>
   </si>
   <si>
@@ -307,9 +253,6 @@
     <t xml:space="preserve">9471492319974</t>
   </si>
   <si>
-    <t xml:space="preserve">https://plus.unsplash.com/premium_photo-1738637796692-d29db83fb7c4?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwzMjV8fHxlbnwwfHx8fHw%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nude the world</t>
   </si>
   <si>
@@ -319,9 +262,6 @@
     <t xml:space="preserve">8578526539056</t>
   </si>
   <si>
-    <t xml:space="preserve">https://plus.unsplash.com/premium_photo-1676422290431-f0d07a64eec5?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwzMzN8fHxlbnwwfHx8fHw%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">Journey Through Time</t>
   </si>
   <si>
@@ -331,9 +271,6 @@
     <t xml:space="preserve">7718640104179</t>
   </si>
   <si>
-    <t xml:space="preserve">https://plus.unsplash.com/premium_photo-1737482089304-3212ccf9a515?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwzMTd8fHxlbnwwfHx8fHw%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">Land or Ocean</t>
   </si>
   <si>
@@ -343,9 +280,6 @@
     <t xml:space="preserve">4831385268452</t>
   </si>
   <si>
-    <t xml:space="preserve">https://plus.unsplash.com/premium_photo-1666266623778-b6ead3081d99?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwyNzN8fHxlbnwwfHx8fHw%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">A gripping novel about a young adventurer who stumbles upon an ancient secret that could change history forever.</t>
   </si>
   <si>
@@ -355,15 +289,9 @@
     <t xml:space="preserve">5094587489675</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1738667379581-a02dd0f0bfe5?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwyODd8fHxlbnwwfHx8fHw%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">2914750700849</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1684262483735-1101bcb10f0d?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwzMDJ8fHxlbnwwfHx8fHw%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">Horizonal line</t>
   </si>
   <si>
@@ -373,147 +301,96 @@
     <t xml:space="preserve">2839769528974</t>
   </si>
   <si>
-    <t xml:space="preserve">https://plus.unsplash.com/premium_photo-1709311438052-9c3f5f867b9a?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwyNjZ8fHxlbnwwfHx8fHw%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">Just Friend</t>
   </si>
   <si>
     <t xml:space="preserve">1993487473398</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1738707060349-c92b5b15bf80?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwyMjl8fHxlbnwwfHx8fHw%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">Baby Baby Poo</t>
   </si>
   <si>
     <t xml:space="preserve">6339843152238</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1738771321771-972e87edffa7?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwyMDh8fHxlbnwwfHx8fHw%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">4980184313763</t>
   </si>
   <si>
-    <t xml:space="preserve">https://plus.unsplash.com/premium_photo-1717279908053-e0e8618eca45?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwyMDJ8fHxlbnwwfHx8fHw%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">Raw on Row</t>
   </si>
   <si>
     <t xml:space="preserve">5766964981365</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1739057736231-3577bfc1a1b9?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwxODh8fHxlbnwwfHx8fHw%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">4843367586294</t>
   </si>
   <si>
-    <t xml:space="preserve">https://plus.unsplash.com/premium_photo-1734549547939-41f90fdf91cf?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwxNzB8fHxlbnwwfHx8fHw%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">Time and Space</t>
   </si>
   <si>
     <t xml:space="preserve">1661836211546</t>
   </si>
   <si>
-    <t xml:space="preserve">https://plus.unsplash.com/premium_photo-1669865742415-596c9a489d77?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwxNjJ8fHxlbnwwfHx8fHw%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">Goods and Products</t>
   </si>
   <si>
     <t xml:space="preserve">3307557524245</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1738468070469-4d92158ffa55?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwxNTV8fHxlbnwwfHx8fHw%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">A wonderful</t>
   </si>
   <si>
     <t xml:space="preserve">4811276399991</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1738253145927-c385871168d8?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwxNTN8fHxlbnwwfHx8fHw%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ping Pong</t>
   </si>
   <si>
     <t xml:space="preserve">9595151983302</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1736354220560-420e5b075881?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwxNDl8fHxlbnwwfHx8fHw%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pode the pole</t>
   </si>
   <si>
     <t xml:space="preserve">2956121747532</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1738168601625-5a472d90952a?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwxMzV8fHxlbnwwfHx8fHw%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">Last Leaf</t>
   </si>
   <si>
     <t xml:space="preserve">1483824784248</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1737917818689-f3b3708de5d7?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwxMjh8fHxlbnwwfHx8fHw%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">Line of Lion</t>
   </si>
   <si>
     <t xml:space="preserve">3387151765062</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1738807991630-260f842bdf49?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwxMTh8fHxlbnwwfHx8fHw%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">War is </t>
   </si>
   <si>
     <t xml:space="preserve">3741334886060</t>
   </si>
   <si>
-    <t xml:space="preserve">https://plus.unsplash.com/premium_photo-1739095638086-f86a16d1a076?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwxMjF8fHxlbnwwfHx8fHw%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">Goody Good</t>
   </si>
   <si>
     <t xml:space="preserve">4148340237683</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1739036462754-6e86520998a2?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwxMDh8fHxlbnwwfHx8fHw%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">The Lotus</t>
   </si>
   <si>
     <t xml:space="preserve">6827851785904</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1739321549350-0357af593300?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwxMDN8fHxlbnwwfHx8fHw%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sunshine</t>
   </si>
   <si>
     <t xml:space="preserve">5281360148072</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1739268377200-43bf019a47b1?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHw5OXx8fGVufDB8fHx8fA%3D%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">Baby Toy</t>
   </si>
   <si>
@@ -523,79 +400,52 @@
     <t xml:space="preserve">Daniel L. Ford</t>
   </si>
   <si>
-    <t xml:space="preserve">https://plus.unsplash.com/premium_photo-1738779001459-3c2efd2f6e88?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHw4OXx8fGVufDB8fHx8fA%3D%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">Historical Lands</t>
   </si>
   <si>
     <t xml:space="preserve">5866738419306</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1739361133037-77be66a4ea6a?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHw4OHx8fGVufDB8fHx8fA%3D%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">God</t>
   </si>
   <si>
     <t xml:space="preserve">9730502118396</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1739403386250-080677ac4c53?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHw3NHx8fGVufDB8fHx8fA%3D%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">Success and Health</t>
   </si>
   <si>
     <t xml:space="preserve">9324439295451</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1739382120560-5b15ad29e3d3?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHw2N3x8fGVufDB8fHx8fA%3D%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">Screening the log</t>
   </si>
   <si>
     <t xml:space="preserve">7353734855899</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1739367156314-cdf4aa3718a5?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHw1Mnx8fGVufDB8fHx8fA%3D%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">The moon and the doom</t>
   </si>
   <si>
     <t xml:space="preserve">8905184457507</t>
   </si>
   <si>
-    <t xml:space="preserve">https://plus.unsplash.com/premium_photo-1739452388443-0292d752dc98?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHw0OXx8fGVufDB8fHx8fA%3D%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">Grid the road</t>
   </si>
   <si>
     <t xml:space="preserve">7599200119414</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1739369484883-4ca5ddea4f29?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwzOHx8fGVufDB8fHx8fA%3D%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">Slat</t>
   </si>
   <si>
     <t xml:space="preserve">3868322715683</t>
   </si>
   <si>
-    <t xml:space="preserve">https://images.unsplash.com/photo-1739381338609-024679941a35?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHw0NHx8fGVufDB8fHx8fA%3D%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">The Hidden Truth</t>
   </si>
   <si>
     <t xml:space="preserve">3044213233560</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://plus.unsplash.com/premium_photo-1738451201702-6099431434d9?w=500&amp;auto=format&amp;fit=crop&amp;q=60&amp;ixlib=rb-4.0.3&amp;ixid=M3wxMjA3fDB8MHxmZWF0dXJlZC1waG90b3MtZmVlZHwzN3x8fGVufDB8fHx8fA%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -760,8 +610,8 @@
   </sheetPr>
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G61" activeCellId="0" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -815,91 +665,83 @@
       <c r="F2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>11</v>
-      </c>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="D3" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>15</v>
       </c>
       <c r="E3" s="8" t="n">
         <v>9</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>17</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="G3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>21</v>
       </c>
       <c r="E4" s="8" t="n">
         <v>3</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>23</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>27</v>
       </c>
       <c r="E5" s="8" t="n">
         <v>9</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>29</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="G5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E6" s="8" t="n">
         <v>4</v>
@@ -907,68 +749,62 @@
       <c r="F6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="9" t="s">
-        <v>34</v>
-      </c>
+      <c r="G6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E7" s="8" t="n">
         <v>10</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>40</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="G7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E8" s="8" t="n">
         <v>1</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>45</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="G8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E9" s="8" t="n">
         <v>4</v>
@@ -976,22 +812,20 @@
       <c r="F9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="9" t="s">
-        <v>49</v>
-      </c>
+      <c r="G9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E10" s="8" t="n">
         <v>10</v>
@@ -999,206 +833,188 @@
       <c r="F10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>54</v>
-      </c>
+      <c r="G10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E11" s="8" t="n">
         <v>8</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>59</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="G11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="E12" s="8" t="n">
         <v>5</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>64</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="G12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="E13" s="8" t="n">
         <v>10</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>69</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="G13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E14" s="8" t="n">
         <v>10</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>73</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="G14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="E15" s="8" t="n">
         <v>6</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>77</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="G15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="E16" s="8" t="n">
         <v>9</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>79</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="G16" s="9"/>
     </row>
     <row r="17" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="E17" s="8" t="n">
         <v>9</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>82</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="G17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E18" s="8" t="n">
         <v>3</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>86</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="G18" s="9"/>
     </row>
     <row r="19" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="E19" s="8" t="n">
         <v>7</v>
@@ -1206,137 +1022,125 @@
       <c r="F19" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G19" s="9" t="s">
-        <v>90</v>
-      </c>
+      <c r="G19" s="9"/>
     </row>
     <row r="20" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="E20" s="8" t="n">
         <v>1</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>95</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="G20" s="9"/>
     </row>
     <row r="21" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="E21" s="8" t="n">
         <v>2</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>63</v>
+      </c>
+      <c r="G21" s="9"/>
+    </row>
+    <row r="22" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="E22" s="8" t="n">
         <v>8</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>53</v>
+      </c>
+      <c r="G22" s="9"/>
+    </row>
+    <row r="23" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="7" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="E23" s="8" t="n">
         <v>9</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>53</v>
+      </c>
+      <c r="G23" s="9"/>
+    </row>
+    <row r="24" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="7" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="E24" s="8" t="n">
         <v>1</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>25</v>
+      </c>
+      <c r="G24" s="9"/>
+    </row>
+    <row r="25" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="E25" s="8" t="n">
         <v>8</v>
@@ -1344,229 +1148,209 @@
       <c r="F25" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G25" s="9" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G25" s="9"/>
+    </row>
+    <row r="26" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="7" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="E26" s="8" t="n">
         <v>1</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>63</v>
+      </c>
+      <c r="G26" s="9"/>
+    </row>
+    <row r="27" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="7" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C27" s="8" t="n">
         <v>33</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="E27" s="8" t="n">
         <v>9</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="G27" s="9" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>49</v>
+      </c>
+      <c r="G27" s="9"/>
+    </row>
+    <row r="28" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="7" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="E28" s="8" t="n">
         <v>2</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>49</v>
+      </c>
+      <c r="G28" s="9"/>
+    </row>
+    <row r="29" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="7" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="E29" s="8" t="n">
         <v>5</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>34</v>
+      </c>
+      <c r="G29" s="9"/>
+    </row>
+    <row r="30" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="7" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>127</v>
+        <v>99</v>
       </c>
       <c r="E30" s="8" t="n">
         <v>1</v>
       </c>
       <c r="F30" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G30" s="9"/>
+    </row>
+    <row r="31" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C31" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G30" s="9" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>32</v>
-      </c>
       <c r="D31" s="7" t="s">
-        <v>129</v>
+        <v>100</v>
       </c>
       <c r="E31" s="8" t="n">
         <v>7</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G31" s="9" t="s">
-        <v>130</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="G31" s="9"/>
     </row>
     <row r="32" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="7" t="s">
-        <v>131</v>
+        <v>101</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="E32" s="8" t="n">
         <v>7</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>133</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="G32" s="9"/>
     </row>
     <row r="33" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="7" t="s">
-        <v>134</v>
+        <v>103</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>135</v>
+        <v>104</v>
       </c>
       <c r="E33" s="8" t="n">
         <v>5</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="G33" s="9" t="s">
-        <v>136</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="G33" s="9"/>
     </row>
     <row r="34" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="7" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
       <c r="E34" s="8" t="n">
         <v>4</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="G34" s="9" t="s">
-        <v>139</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="G34" s="9"/>
     </row>
     <row r="35" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="7" t="s">
-        <v>140</v>
+        <v>107</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>141</v>
+        <v>108</v>
       </c>
       <c r="E35" s="8" t="n">
         <v>2</v>
@@ -1574,137 +1358,125 @@
       <c r="F35" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G35" s="9" t="s">
-        <v>142</v>
-      </c>
+      <c r="G35" s="9"/>
     </row>
     <row r="36" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="7" t="s">
-        <v>143</v>
+        <v>109</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="E36" s="8" t="n">
         <v>1</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="G36" s="9" t="s">
-        <v>145</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="G36" s="9"/>
     </row>
     <row r="37" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="7" t="s">
-        <v>146</v>
+        <v>111</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>147</v>
+        <v>112</v>
       </c>
       <c r="E37" s="8" t="n">
         <v>4</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G37" s="9" t="s">
-        <v>148</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="G37" s="9"/>
     </row>
     <row r="38" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="7" t="s">
-        <v>149</v>
+        <v>113</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="E38" s="8" t="n">
         <v>9</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G38" s="9" t="s">
-        <v>151</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="G38" s="9"/>
     </row>
     <row r="39" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="7" t="s">
-        <v>152</v>
+        <v>115</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>153</v>
+        <v>116</v>
       </c>
       <c r="E39" s="8" t="n">
         <v>5</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G39" s="9" t="s">
-        <v>154</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="G39" s="9"/>
     </row>
     <row r="40" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="7" t="s">
-        <v>155</v>
+        <v>117</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>156</v>
+        <v>118</v>
       </c>
       <c r="E40" s="8" t="n">
         <v>8</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G40" s="9" t="s">
-        <v>157</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="G40" s="9"/>
     </row>
     <row r="41" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="7" t="s">
-        <v>158</v>
+        <v>119</v>
       </c>
       <c r="B41" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C41" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C41" s="10" t="s">
-        <v>61</v>
-      </c>
       <c r="D41" s="7" t="s">
-        <v>159</v>
+        <v>120</v>
       </c>
       <c r="E41" s="8" t="n">
         <v>2</v>
@@ -1712,229 +1484,209 @@
       <c r="F41" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G41" s="9" t="s">
-        <v>160</v>
-      </c>
+      <c r="G41" s="9"/>
     </row>
     <row r="42" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="7" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>162</v>
+        <v>122</v>
       </c>
       <c r="E42" s="8" t="n">
         <v>6</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G42" s="9" t="s">
-        <v>163</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="G42" s="9"/>
     </row>
     <row r="43" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="7" t="s">
-        <v>164</v>
+        <v>123</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="E43" s="8" t="n">
         <v>7</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="G43" s="9" t="s">
-        <v>167</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="G43" s="9"/>
     </row>
     <row r="44" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="7" t="s">
-        <v>168</v>
+        <v>126</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>169</v>
+        <v>127</v>
       </c>
       <c r="E44" s="8" t="n">
         <v>5</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="G44" s="9" t="s">
-        <v>170</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="G44" s="9"/>
     </row>
     <row r="45" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="7" t="s">
-        <v>171</v>
+        <v>128</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>172</v>
+        <v>129</v>
       </c>
       <c r="E45" s="8" t="n">
         <v>4</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="G45" s="9" t="s">
-        <v>173</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="G45" s="9"/>
     </row>
     <row r="46" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="7" t="s">
-        <v>174</v>
+        <v>130</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>175</v>
+        <v>131</v>
       </c>
       <c r="E46" s="8" t="n">
         <v>3</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G46" s="9" t="s">
-        <v>176</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="G46" s="9"/>
     </row>
     <row r="47" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="7" t="s">
-        <v>177</v>
+        <v>132</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>178</v>
+        <v>133</v>
       </c>
       <c r="E47" s="8" t="n">
         <v>4</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="G47" s="9" t="s">
-        <v>179</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="G47" s="9"/>
     </row>
     <row r="48" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="7" t="s">
-        <v>180</v>
+        <v>134</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>181</v>
+        <v>135</v>
       </c>
       <c r="E48" s="8" t="n">
         <v>2</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="G48" s="9" t="s">
-        <v>182</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="G48" s="9"/>
     </row>
     <row r="49" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="7" t="s">
-        <v>183</v>
+        <v>136</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>184</v>
+        <v>137</v>
       </c>
       <c r="E49" s="8" t="n">
         <v>4</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="G49" s="9" t="s">
-        <v>185</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="G49" s="9"/>
     </row>
     <row r="50" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="7" t="s">
-        <v>186</v>
+        <v>138</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>187</v>
+        <v>139</v>
       </c>
       <c r="E50" s="8" t="n">
         <v>9</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="G50" s="9" t="s">
-        <v>188</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="G50" s="9"/>
     </row>
     <row r="51" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="7" t="s">
-        <v>189</v>
+        <v>140</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>190</v>
+        <v>141</v>
       </c>
       <c r="E51" s="8" t="n">
         <v>6</v>
@@ -1942,9 +1694,7 @@
       <c r="F51" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G51" s="9" t="s">
-        <v>191</v>
-      </c>
+      <c r="G51" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>